<commit_message>
Fixes of Test Cases of lesson 4
</commit_message>
<xml_diff>
--- a/AndyTEST/Libs/SimpleScenariosChecklist_02.xlsx
+++ b/AndyTEST/Libs/SimpleScenariosChecklist_02.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="airports" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="915">
   <si>
     <t>Airports</t>
   </si>
@@ -2299,9 +2299,6 @@
   </si>
   <si>
     <t>Check the airline of flight #1035</t>
-  </si>
-  <si>
-    <t>SELECT flightNumber FROM Airlines</t>
   </si>
   <si>
     <t xml:space="preserve">1001;1002;1003;1004;1005;1006;1007;1008;1009;1010;1011;1012;1013;1014;1015;1016;1017;1018;1019;1020;1021;1022;1023;1024;1025;1026;1027;1028;1029;1030;1031;1032;1033;1034;1035;
@@ -2759,6 +2756,12 @@
   </si>
   <si>
     <t>SELECT isMealincluded FROM Airlines WHERE flightNumber = 1001;</t>
+  </si>
+  <si>
+    <t>London;Paris;Sydney;Berlin;Munich;New-York;Kiev;Budapest;Beijing;Prague;Helsinki;Ottava;Vilnius;Milan;Barcelona;</t>
+  </si>
+  <si>
+    <t>SELECT flightNumber FROM Airlines;</t>
   </si>
 </sst>
 </file>
@@ -2882,7 +2885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2964,15 +2967,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3034,6 +3028,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3081,7 +3078,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3116,7 +3113,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3328,17 +3325,17 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="C3" sqref="C3:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="57.375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="23.5" style="9" customWidth="1"/>
-    <col min="4" max="4" width="13.625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="17.875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="16.625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -3384,8 +3381,10 @@
       <c r="D3" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="36"/>
+      <c r="E3" s="30" t="s">
+        <v>913</v>
+      </c>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -3396,8 +3395,8 @@
       </c>
       <c r="C4" s="28"/>
       <c r="D4" s="31"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="37"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -3408,8 +3407,8 @@
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="31"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -3420,8 +3419,8 @@
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="31"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="37"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -3432,8 +3431,8 @@
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="31"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="37"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -3444,8 +3443,8 @@
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="31"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -3456,8 +3455,8 @@
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="31"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="37"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -3468,8 +3467,8 @@
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="31"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -3480,8 +3479,8 @@
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="31"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -3492,8 +3491,8 @@
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="31"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="37"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -3504,8 +3503,8 @@
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="31"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -3516,8 +3515,8 @@
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="31"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="37"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -3528,8 +3527,8 @@
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="31"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="37"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -3540,8 +3539,8 @@
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="31"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="37"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -3552,8 +3551,8 @@
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="32"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="38"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -4054,18 +4053,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="54.25" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
@@ -4098,7 +4097,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="22" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4114,7 +4113,7 @@
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
     </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -4130,7 +4129,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -4146,7 +4145,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -4162,7 +4161,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -4178,7 +4177,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -4194,7 +4193,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -4210,7 +4209,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -4226,7 +4225,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -4242,7 +4241,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -4306,7 +4305,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -4322,7 +4321,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -4338,7 +4337,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -4354,7 +4353,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -4370,7 +4369,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -4386,7 +4385,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -4402,7 +4401,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -4418,7 +4417,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -4434,7 +4433,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -4450,7 +4449,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -4466,7 +4465,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -4482,7 +4481,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -4498,7 +4497,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -4514,7 +4513,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -4530,7 +4529,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -4546,7 +4545,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -4562,7 +4561,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -4594,7 +4593,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -4610,7 +4609,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -4626,7 +4625,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -4642,7 +4641,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -5218,7 +5217,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -5234,7 +5233,7 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -5250,7 +5249,7 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -5266,7 +5265,7 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -5282,7 +5281,7 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -5298,7 +5297,7 @@
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -5314,7 +5313,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -5330,7 +5329,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -5346,7 +5345,7 @@
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -5362,7 +5361,7 @@
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -5378,7 +5377,7 @@
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>81</v>
       </c>
@@ -5394,7 +5393,7 @@
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -5410,7 +5409,7 @@
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -5426,7 +5425,7 @@
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -5442,7 +5441,7 @@
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>85</v>
       </c>
@@ -5458,7 +5457,7 @@
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>86</v>
       </c>
@@ -5474,7 +5473,7 @@
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>87</v>
       </c>
@@ -5490,7 +5489,7 @@
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>88</v>
       </c>
@@ -5506,7 +5505,7 @@
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>89</v>
       </c>
@@ -5522,7 +5521,7 @@
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -5538,7 +5537,7 @@
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -5554,7 +5553,7 @@
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -5570,7 +5569,7 @@
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -5586,7 +5585,7 @@
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -5602,7 +5601,7 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -5618,7 +5617,7 @@
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>96</v>
       </c>
@@ -5634,7 +5633,7 @@
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -5650,7 +5649,7 @@
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -5666,7 +5665,7 @@
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -5682,7 +5681,7 @@
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -5698,7 +5697,7 @@
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -5714,7 +5713,7 @@
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -5730,7 +5729,7 @@
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>103</v>
       </c>
@@ -5746,7 +5745,7 @@
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>104</v>
       </c>
@@ -5762,7 +5761,7 @@
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
     </row>
-    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>105</v>
       </c>
@@ -5778,7 +5777,7 @@
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>106</v>
       </c>
@@ -5794,7 +5793,7 @@
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
     </row>
-    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>107</v>
       </c>
@@ -5810,7 +5809,7 @@
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
     </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>108</v>
       </c>
@@ -5826,7 +5825,7 @@
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
     </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>109</v>
       </c>
@@ -5842,7 +5841,7 @@
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
     </row>
-    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>110</v>
       </c>
@@ -5858,7 +5857,7 @@
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>111</v>
       </c>
@@ -5874,7 +5873,7 @@
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>112</v>
       </c>
@@ -5890,7 +5889,7 @@
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>113</v>
       </c>
@@ -5906,7 +5905,7 @@
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
     </row>
-    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>114</v>
       </c>
@@ -5922,7 +5921,7 @@
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
     </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>115</v>
       </c>
@@ -5938,7 +5937,7 @@
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
     </row>
-    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>116</v>
       </c>
@@ -5954,7 +5953,7 @@
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
     </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A119" s="5">
         <v>117</v>
       </c>
@@ -5970,7 +5969,7 @@
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
     </row>
-    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>118</v>
       </c>
@@ -5986,7 +5985,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
     </row>
-    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>119</v>
       </c>
@@ -6002,7 +6001,7 @@
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
     </row>
-    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>120</v>
       </c>
@@ -6018,7 +6017,7 @@
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
     </row>
-    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="5">
         <v>121</v>
       </c>
@@ -6034,7 +6033,7 @@
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
     </row>
-    <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>122</v>
       </c>
@@ -6050,7 +6049,7 @@
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
     </row>
-    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>123</v>
       </c>
@@ -6066,7 +6065,7 @@
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
     </row>
-    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>124</v>
       </c>
@@ -6082,7 +6081,7 @@
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
     </row>
-    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>125</v>
       </c>
@@ -6098,7 +6097,7 @@
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
     </row>
-    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>126</v>
       </c>
@@ -6114,7 +6113,7 @@
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
     </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
         <v>127</v>
       </c>
@@ -6130,7 +6129,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
     </row>
-    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>128</v>
       </c>
@@ -6146,7 +6145,7 @@
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
     </row>
-    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>129</v>
       </c>
@@ -6162,7 +6161,7 @@
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
     </row>
-    <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>130</v>
       </c>
@@ -6178,7 +6177,7 @@
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
     </row>
-    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>131</v>
       </c>
@@ -6194,7 +6193,7 @@
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>132</v>
       </c>
@@ -6210,7 +6209,7 @@
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
     </row>
-    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="5">
         <v>133</v>
       </c>
@@ -6226,7 +6225,7 @@
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>
     </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>134</v>
       </c>
@@ -6242,7 +6241,7 @@
       <c r="E136" s="2"/>
       <c r="F136" s="2"/>
     </row>
-    <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="5">
         <v>135</v>
       </c>
@@ -6258,7 +6257,7 @@
       <c r="E137" s="2"/>
       <c r="F137" s="2"/>
     </row>
-    <row r="138" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>136</v>
       </c>
@@ -6274,7 +6273,7 @@
       <c r="E138" s="2"/>
       <c r="F138" s="2"/>
     </row>
-    <row r="139" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
         <v>137</v>
       </c>
@@ -6290,7 +6289,7 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
     </row>
-    <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>138</v>
       </c>
@@ -6306,7 +6305,7 @@
       <c r="E140" s="2"/>
       <c r="F140" s="2"/>
     </row>
-    <row r="141" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="5">
         <v>139</v>
       </c>
@@ -6322,7 +6321,7 @@
       <c r="E141" s="2"/>
       <c r="F141" s="2"/>
     </row>
-    <row r="142" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>140</v>
       </c>
@@ -6898,7 +6897,7 @@
       <c r="E177" s="2"/>
       <c r="F177" s="2"/>
     </row>
-    <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="5">
         <v>176</v>
       </c>
@@ -6914,7 +6913,7 @@
       <c r="E178" s="2"/>
       <c r="F178" s="2"/>
     </row>
-    <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="5">
         <v>177</v>
       </c>
@@ -6930,7 +6929,7 @@
       <c r="E179" s="2"/>
       <c r="F179" s="2"/>
     </row>
-    <row r="180" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A180" s="5">
         <v>178</v>
       </c>
@@ -6946,7 +6945,7 @@
       <c r="E180" s="2"/>
       <c r="F180" s="2"/>
     </row>
-    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="5">
         <v>179</v>
       </c>
@@ -6962,7 +6961,7 @@
       <c r="E181" s="2"/>
       <c r="F181" s="2"/>
     </row>
-    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A182" s="5">
         <v>180</v>
       </c>
@@ -6978,7 +6977,7 @@
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
     </row>
-    <row r="183" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A183" s="5">
         <v>181</v>
       </c>
@@ -6994,7 +6993,7 @@
       <c r="E183" s="2"/>
       <c r="F183" s="2"/>
     </row>
-    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" s="5">
         <v>182</v>
       </c>
@@ -7010,7 +7009,7 @@
       <c r="E184" s="2"/>
       <c r="F184" s="2"/>
     </row>
-    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A185" s="5">
         <v>183</v>
       </c>
@@ -7026,7 +7025,7 @@
       <c r="E185" s="2"/>
       <c r="F185" s="2"/>
     </row>
-    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="5">
         <v>184</v>
       </c>
@@ -7042,7 +7041,7 @@
       <c r="E186" s="2"/>
       <c r="F186" s="2"/>
     </row>
-    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="5">
         <v>185</v>
       </c>
@@ -7058,7 +7057,7 @@
       <c r="E187" s="2"/>
       <c r="F187" s="2"/>
     </row>
-    <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" s="5">
         <v>186</v>
       </c>
@@ -7074,7 +7073,7 @@
       <c r="E188" s="2"/>
       <c r="F188" s="2"/>
     </row>
-    <row r="189" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="5">
         <v>187</v>
       </c>
@@ -7090,7 +7089,7 @@
       <c r="E189" s="2"/>
       <c r="F189" s="2"/>
     </row>
-    <row r="190" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A190" s="5">
         <v>188</v>
       </c>
@@ -7106,7 +7105,7 @@
       <c r="E190" s="2"/>
       <c r="F190" s="2"/>
     </row>
-    <row r="191" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A191" s="5">
         <v>189</v>
       </c>
@@ -7122,7 +7121,7 @@
       <c r="E191" s="2"/>
       <c r="F191" s="2"/>
     </row>
-    <row r="192" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="5">
         <v>190</v>
       </c>
@@ -7138,7 +7137,7 @@
       <c r="E192" s="2"/>
       <c r="F192" s="2"/>
     </row>
-    <row r="193" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="5">
         <v>191</v>
       </c>
@@ -7154,7 +7153,7 @@
       <c r="E193" s="2"/>
       <c r="F193" s="2"/>
     </row>
-    <row r="194" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A194" s="5">
         <v>192</v>
       </c>
@@ -7170,7 +7169,7 @@
       <c r="E194" s="2"/>
       <c r="F194" s="2"/>
     </row>
-    <row r="195" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A195" s="5">
         <v>193</v>
       </c>
@@ -7186,7 +7185,7 @@
       <c r="E195" s="2"/>
       <c r="F195" s="2"/>
     </row>
-    <row r="196" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="5">
         <v>194</v>
       </c>
@@ -7202,7 +7201,7 @@
       <c r="E196" s="2"/>
       <c r="F196" s="2"/>
     </row>
-    <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" s="5">
         <v>195</v>
       </c>
@@ -7218,7 +7217,7 @@
       <c r="E197" s="2"/>
       <c r="F197" s="2"/>
     </row>
-    <row r="198" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A198" s="5">
         <v>196</v>
       </c>
@@ -7234,7 +7233,7 @@
       <c r="E198" s="2"/>
       <c r="F198" s="2"/>
     </row>
-    <row r="199" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A199" s="5">
         <v>197</v>
       </c>
@@ -7250,7 +7249,7 @@
       <c r="E199" s="2"/>
       <c r="F199" s="2"/>
     </row>
-    <row r="200" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A200" s="5">
         <v>198</v>
       </c>
@@ -7266,7 +7265,7 @@
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
     </row>
-    <row r="201" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A201" s="5">
         <v>199</v>
       </c>
@@ -7282,7 +7281,7 @@
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
     </row>
-    <row r="202" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A202" s="5">
         <v>200</v>
       </c>
@@ -7298,7 +7297,7 @@
       <c r="E202" s="2"/>
       <c r="F202" s="2"/>
     </row>
-    <row r="203" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A203" s="5">
         <v>201</v>
       </c>
@@ -7314,7 +7313,7 @@
       <c r="E203" s="2"/>
       <c r="F203" s="2"/>
     </row>
-    <row r="204" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A204" s="5">
         <v>202</v>
       </c>
@@ -7330,7 +7329,7 @@
       <c r="E204" s="2"/>
       <c r="F204" s="2"/>
     </row>
-    <row r="205" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A205" s="5">
         <v>203</v>
       </c>
@@ -7346,7 +7345,7 @@
       <c r="E205" s="2"/>
       <c r="F205" s="2"/>
     </row>
-    <row r="206" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A206" s="5">
         <v>204</v>
       </c>
@@ -7362,7 +7361,7 @@
       <c r="E206" s="2"/>
       <c r="F206" s="2"/>
     </row>
-    <row r="207" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="5">
         <v>205</v>
       </c>
@@ -7378,7 +7377,7 @@
       <c r="E207" s="2"/>
       <c r="F207" s="2"/>
     </row>
-    <row r="208" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A208" s="5">
         <v>206</v>
       </c>
@@ -7394,7 +7393,7 @@
       <c r="E208" s="2"/>
       <c r="F208" s="2"/>
     </row>
-    <row r="209" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A209" s="5">
         <v>207</v>
       </c>
@@ -7410,7 +7409,7 @@
       <c r="E209" s="2"/>
       <c r="F209" s="2"/>
     </row>
-    <row r="210" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A210" s="5">
         <v>208</v>
       </c>
@@ -7426,7 +7425,7 @@
       <c r="E210" s="2"/>
       <c r="F210" s="2"/>
     </row>
-    <row r="211" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" s="5">
         <v>209</v>
       </c>
@@ -7442,7 +7441,7 @@
       <c r="E211" s="2"/>
       <c r="F211" s="2"/>
     </row>
-    <row r="212" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A212" s="5">
         <v>210</v>
       </c>
@@ -7519,18 +7518,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F177"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="55" style="9" customWidth="1"/>
-    <col min="3" max="3" width="25.25" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="19.375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
@@ -7570,14 +7569,14 @@
       <c r="B3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="36" t="s">
+        <v>914</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>761</v>
       </c>
-      <c r="D3" s="42" t="s">
-        <v>762</v>
-      </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="48"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -7586,10 +7585,10 @@
       <c r="B4" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="49"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -7598,10 +7597,10 @@
       <c r="B5" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="49"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="46"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -7610,10 +7609,10 @@
       <c r="B6" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="49"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="46"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -7622,10 +7621,10 @@
       <c r="B7" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="49"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="46"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -7634,10 +7633,10 @@
       <c r="B8" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="49"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="46"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -7646,10 +7645,10 @@
       <c r="B9" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="49"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="46"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -7658,10 +7657,10 @@
       <c r="B10" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="49"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="46"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -7670,10 +7669,10 @@
       <c r="B11" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="49"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="46"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -7682,10 +7681,10 @@
       <c r="B12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="49"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="46"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -7694,10 +7693,10 @@
       <c r="B13" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="49"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -7706,10 +7705,10 @@
       <c r="B14" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="49"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="46"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -7718,10 +7717,10 @@
       <c r="B15" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="49"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="46"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -7730,10 +7729,10 @@
       <c r="B16" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="49"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -7742,10 +7741,10 @@
       <c r="B17" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="49"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -7754,10 +7753,10 @@
       <c r="B18" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="49"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="46"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -7766,10 +7765,10 @@
       <c r="B19" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="49"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="46"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -7778,10 +7777,10 @@
       <c r="B20" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="49"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="46"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -7790,10 +7789,10 @@
       <c r="B21" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="49"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -7802,10 +7801,10 @@
       <c r="B22" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="49"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -7814,10 +7813,10 @@
       <c r="B23" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="49"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="46"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -7826,10 +7825,10 @@
       <c r="B24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="49"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="46"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -7838,10 +7837,10 @@
       <c r="B25" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="49"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="46"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -7850,10 +7849,10 @@
       <c r="B26" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="49"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="46"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -7862,10 +7861,10 @@
       <c r="B27" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="49"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="46"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -7874,10 +7873,10 @@
       <c r="B28" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="49"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="46"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -7886,10 +7885,10 @@
       <c r="B29" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="49"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="46"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -7898,10 +7897,10 @@
       <c r="B30" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="49"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="46"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -7910,10 +7909,10 @@
       <c r="B31" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="49"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="46"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -7922,10 +7921,10 @@
       <c r="B32" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="49"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="46"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -7934,10 +7933,10 @@
       <c r="B33" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="49"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="46"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
@@ -7946,10 +7945,10 @@
       <c r="B34" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="49"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="46"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
@@ -7958,10 +7957,10 @@
       <c r="B35" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C35" s="40"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="49"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="46"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
@@ -7970,10 +7969,10 @@
       <c r="B36" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="49"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="46"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
@@ -7982,12 +7981,12 @@
       <c r="B37" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="50"/>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C37" s="38"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="47"/>
+    </row>
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -7995,15 +7994,15 @@
         <v>726</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E38" s="24"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -8011,15 +8010,15 @@
         <v>727</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -8027,15 +8026,15 @@
         <v>728</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E40" s="24"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -8043,15 +8042,15 @@
         <v>729</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -8059,15 +8058,15 @@
         <v>730</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -8075,15 +8074,15 @@
         <v>731</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E43" s="24"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -8091,15 +8090,15 @@
         <v>732</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E44" s="24"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -8107,15 +8106,15 @@
         <v>733</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -8123,15 +8122,15 @@
         <v>734</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E46" s="24"/>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -8139,15 +8138,15 @@
         <v>735</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E47" s="24"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>46</v>
       </c>
@@ -8155,15 +8154,15 @@
         <v>736</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E48" s="24"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>47</v>
       </c>
@@ -8171,15 +8170,15 @@
         <v>737</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E49" s="24"/>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>48</v>
       </c>
@@ -8187,15 +8186,15 @@
         <v>738</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E50" s="24"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>49</v>
       </c>
@@ -8203,15 +8202,15 @@
         <v>739</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E51" s="24"/>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>50</v>
       </c>
@@ -8219,15 +8218,15 @@
         <v>740</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E52" s="24"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>51</v>
       </c>
@@ -8235,15 +8234,15 @@
         <v>741</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E53" s="24"/>
       <c r="F53" s="2"/>
     </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>52</v>
       </c>
@@ -8251,15 +8250,15 @@
         <v>742</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E54" s="24"/>
       <c r="F54" s="2"/>
     </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>53</v>
       </c>
@@ -8267,15 +8266,15 @@
         <v>743</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E55" s="24"/>
       <c r="F55" s="2"/>
     </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>54</v>
       </c>
@@ -8283,15 +8282,15 @@
         <v>744</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E56" s="24"/>
       <c r="F56" s="2"/>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>55</v>
       </c>
@@ -8299,15 +8298,15 @@
         <v>745</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="2"/>
     </row>
-    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>56</v>
       </c>
@@ -8315,15 +8314,15 @@
         <v>746</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E58" s="24"/>
       <c r="F58" s="2"/>
     </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>57</v>
       </c>
@@ -8331,15 +8330,15 @@
         <v>747</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E59" s="24"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>58</v>
       </c>
@@ -8347,15 +8346,15 @@
         <v>748</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E60" s="24"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>59</v>
       </c>
@@ -8363,15 +8362,15 @@
         <v>749</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E61" s="24"/>
       <c r="F61" s="2"/>
     </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>60</v>
       </c>
@@ -8379,15 +8378,15 @@
         <v>750</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E62" s="24"/>
       <c r="F62" s="2"/>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>61</v>
       </c>
@@ -8395,15 +8394,15 @@
         <v>751</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E63" s="24"/>
       <c r="F63" s="2"/>
     </row>
-    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>62</v>
       </c>
@@ -8411,15 +8410,15 @@
         <v>752</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E64" s="24"/>
       <c r="F64" s="2"/>
     </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>63</v>
       </c>
@@ -8427,15 +8426,15 @@
         <v>753</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E65" s="24"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>64</v>
       </c>
@@ -8443,15 +8442,15 @@
         <v>754</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E66" s="24"/>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>65</v>
       </c>
@@ -8459,15 +8458,15 @@
         <v>755</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E67" s="24"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>66</v>
       </c>
@@ -8475,15 +8474,15 @@
         <v>756</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E68" s="24"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>67</v>
       </c>
@@ -8491,15 +8490,15 @@
         <v>757</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E69" s="24"/>
       <c r="F69" s="2"/>
     </row>
-    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -8507,15 +8506,15 @@
         <v>758</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E70" s="24"/>
       <c r="F70" s="2"/>
     </row>
-    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>69</v>
       </c>
@@ -8523,15 +8522,15 @@
         <v>759</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E71" s="24"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>70</v>
       </c>
@@ -8539,15 +8538,15 @@
         <v>760</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E72" s="24"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>71</v>
       </c>
@@ -8555,7 +8554,7 @@
         <v>84</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>206</v>
@@ -8563,7 +8562,7 @@
       <c r="E73" s="17"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>72</v>
       </c>
@@ -8571,7 +8570,7 @@
         <v>87</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>239</v>
@@ -8579,7 +8578,7 @@
       <c r="E74" s="17"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>73</v>
       </c>
@@ -8587,7 +8586,7 @@
         <v>197</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>239</v>
@@ -8595,7 +8594,7 @@
       <c r="E75" s="17"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>74</v>
       </c>
@@ -8603,7 +8602,7 @@
         <v>92</v>
       </c>
       <c r="C76" s="23" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>206</v>
@@ -8611,7 +8610,7 @@
       <c r="E76" s="17"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>75</v>
       </c>
@@ -8619,7 +8618,7 @@
         <v>95</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>239</v>
@@ -8627,7 +8626,7 @@
       <c r="E77" s="17"/>
       <c r="F77" s="2"/>
     </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>76</v>
       </c>
@@ -8635,7 +8634,7 @@
         <v>98</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>206</v>
@@ -8643,7 +8642,7 @@
       <c r="E78" s="17"/>
       <c r="F78" s="2"/>
     </row>
-    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>77</v>
       </c>
@@ -8651,7 +8650,7 @@
         <v>102</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>206</v>
@@ -8659,7 +8658,7 @@
       <c r="E79" s="17"/>
       <c r="F79" s="2"/>
     </row>
-    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>78</v>
       </c>
@@ -8667,7 +8666,7 @@
         <v>105</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>206</v>
@@ -8675,7 +8674,7 @@
       <c r="E80" s="17"/>
       <c r="F80" s="2"/>
     </row>
-    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>79</v>
       </c>
@@ -8683,7 +8682,7 @@
         <v>108</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>239</v>
@@ -8691,7 +8690,7 @@
       <c r="E81" s="17"/>
       <c r="F81" s="2"/>
     </row>
-    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>80</v>
       </c>
@@ -8699,7 +8698,7 @@
         <v>112</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>239</v>
@@ -8707,7 +8706,7 @@
       <c r="E82" s="17"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>81</v>
       </c>
@@ -8715,7 +8714,7 @@
         <v>115</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>206</v>
@@ -8723,7 +8722,7 @@
       <c r="E83" s="17"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>82</v>
       </c>
@@ -8731,7 +8730,7 @@
         <v>119</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>239</v>
@@ -8739,7 +8738,7 @@
       <c r="E84" s="17"/>
       <c r="F84" s="2"/>
     </row>
-    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>83</v>
       </c>
@@ -8747,7 +8746,7 @@
         <v>123</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>239</v>
@@ -8755,7 +8754,7 @@
       <c r="E85" s="17"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>84</v>
       </c>
@@ -8763,7 +8762,7 @@
         <v>127</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>239</v>
@@ -8771,7 +8770,7 @@
       <c r="E86" s="17"/>
       <c r="F86" s="2"/>
     </row>
-    <row r="87" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>85</v>
       </c>
@@ -8779,7 +8778,7 @@
         <v>130</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>206</v>
@@ -8787,7 +8786,7 @@
       <c r="E87" s="17"/>
       <c r="F87" s="2"/>
     </row>
-    <row r="88" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>86</v>
       </c>
@@ -8795,7 +8794,7 @@
         <v>133</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>206</v>
@@ -8803,7 +8802,7 @@
       <c r="E88" s="17"/>
       <c r="F88" s="2"/>
     </row>
-    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>87</v>
       </c>
@@ -8811,7 +8810,7 @@
         <v>136</v>
       </c>
       <c r="C89" s="23" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>239</v>
@@ -8819,7 +8818,7 @@
       <c r="E89" s="17"/>
       <c r="F89" s="2"/>
     </row>
-    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>88</v>
       </c>
@@ -8827,7 +8826,7 @@
         <v>140</v>
       </c>
       <c r="C90" s="23" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>206</v>
@@ -8835,7 +8834,7 @@
       <c r="E90" s="17"/>
       <c r="F90" s="2"/>
     </row>
-    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>89</v>
       </c>
@@ -8843,7 +8842,7 @@
         <v>144</v>
       </c>
       <c r="C91" s="23" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>239</v>
@@ -8851,7 +8850,7 @@
       <c r="E91" s="17"/>
       <c r="F91" s="2"/>
     </row>
-    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>90</v>
       </c>
@@ -8859,7 +8858,7 @@
         <v>147</v>
       </c>
       <c r="C92" s="23" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>206</v>
@@ -8867,7 +8866,7 @@
       <c r="E92" s="17"/>
       <c r="F92" s="2"/>
     </row>
-    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>91</v>
       </c>
@@ -8875,7 +8874,7 @@
         <v>150</v>
       </c>
       <c r="C93" s="23" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>239</v>
@@ -8883,7 +8882,7 @@
       <c r="E93" s="17"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>92</v>
       </c>
@@ -8891,7 +8890,7 @@
         <v>153</v>
       </c>
       <c r="C94" s="23" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>239</v>
@@ -8899,7 +8898,7 @@
       <c r="E94" s="17"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>93</v>
       </c>
@@ -8907,7 +8906,7 @@
         <v>155</v>
       </c>
       <c r="C95" s="23" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>206</v>
@@ -8915,7 +8914,7 @@
       <c r="E95" s="17"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>94</v>
       </c>
@@ -8923,7 +8922,7 @@
         <v>158</v>
       </c>
       <c r="C96" s="23" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>239</v>
@@ -8931,7 +8930,7 @@
       <c r="E96" s="17"/>
       <c r="F96" s="2"/>
     </row>
-    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>95</v>
       </c>
@@ -8939,7 +8938,7 @@
         <v>161</v>
       </c>
       <c r="C97" s="23" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>206</v>
@@ -8947,7 +8946,7 @@
       <c r="E97" s="17"/>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>96</v>
       </c>
@@ -8955,7 +8954,7 @@
         <v>164</v>
       </c>
       <c r="C98" s="23" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>206</v>
@@ -8963,7 +8962,7 @@
       <c r="E98" s="17"/>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>97</v>
       </c>
@@ -8971,7 +8970,7 @@
         <v>168</v>
       </c>
       <c r="C99" s="23" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>239</v>
@@ -8979,7 +8978,7 @@
       <c r="E99" s="17"/>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>98</v>
       </c>
@@ -8987,7 +8986,7 @@
         <v>171</v>
       </c>
       <c r="C100" s="23" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>239</v>
@@ -8995,7 +8994,7 @@
       <c r="E100" s="17"/>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>99</v>
       </c>
@@ -9003,7 +9002,7 @@
         <v>175</v>
       </c>
       <c r="C101" s="23" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>206</v>
@@ -9011,7 +9010,7 @@
       <c r="E101" s="17"/>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>100</v>
       </c>
@@ -9019,7 +9018,7 @@
         <v>179</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>206</v>
@@ -9027,7 +9026,7 @@
       <c r="E102" s="17"/>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
         <v>101</v>
       </c>
@@ -9035,7 +9034,7 @@
         <v>182</v>
       </c>
       <c r="C103" s="23" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>206</v>
@@ -9043,7 +9042,7 @@
       <c r="E103" s="17"/>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>102</v>
       </c>
@@ -9051,7 +9050,7 @@
         <v>185</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>206</v>
@@ -9059,7 +9058,7 @@
       <c r="E104" s="17"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>103</v>
       </c>
@@ -9067,7 +9066,7 @@
         <v>188</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>239</v>
@@ -9075,7 +9074,7 @@
       <c r="E105" s="17"/>
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>104</v>
       </c>
@@ -9083,7 +9082,7 @@
         <v>191</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>239</v>
@@ -9091,7 +9090,7 @@
       <c r="E106" s="17"/>
       <c r="F106" s="2"/>
     </row>
-    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>105</v>
       </c>
@@ -9099,7 +9098,7 @@
         <v>194</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>239</v>
@@ -9115,7 +9114,7 @@
         <v>85</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>239</v>
@@ -9131,7 +9130,7 @@
         <v>88</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>239</v>
@@ -9147,7 +9146,7 @@
         <v>198</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>206</v>
@@ -9163,7 +9162,7 @@
         <v>93</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>206</v>
@@ -9179,7 +9178,7 @@
         <v>96</v>
       </c>
       <c r="C112" s="23" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>239</v>
@@ -9195,7 +9194,7 @@
         <v>99</v>
       </c>
       <c r="C113" s="23" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>239</v>
@@ -9211,7 +9210,7 @@
         <v>103</v>
       </c>
       <c r="C114" s="23" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>239</v>
@@ -9227,7 +9226,7 @@
         <v>106</v>
       </c>
       <c r="C115" s="23" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>239</v>
@@ -9243,7 +9242,7 @@
         <v>109</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>239</v>
@@ -9259,7 +9258,7 @@
         <v>113</v>
       </c>
       <c r="C117" s="23" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>206</v>
@@ -9275,7 +9274,7 @@
         <v>116</v>
       </c>
       <c r="C118" s="23" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>206</v>
@@ -9291,7 +9290,7 @@
         <v>120</v>
       </c>
       <c r="C119" s="23" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>206</v>
@@ -9307,7 +9306,7 @@
         <v>124</v>
       </c>
       <c r="C120" s="23" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>206</v>
@@ -9323,7 +9322,7 @@
         <v>128</v>
       </c>
       <c r="C121" s="23" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>206</v>
@@ -9339,7 +9338,7 @@
         <v>131</v>
       </c>
       <c r="C122" s="23" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>239</v>
@@ -9355,7 +9354,7 @@
         <v>134</v>
       </c>
       <c r="C123" s="23" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>206</v>
@@ -9371,7 +9370,7 @@
         <v>137</v>
       </c>
       <c r="C124" s="23" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>239</v>
@@ -9387,7 +9386,7 @@
         <v>141</v>
       </c>
       <c r="C125" s="23" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>206</v>
@@ -9403,7 +9402,7 @@
         <v>145</v>
       </c>
       <c r="C126" s="23" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>239</v>
@@ -9419,7 +9418,7 @@
         <v>148</v>
       </c>
       <c r="C127" s="23" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>239</v>
@@ -9435,7 +9434,7 @@
         <v>151</v>
       </c>
       <c r="C128" s="23" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>239</v>
@@ -9451,7 +9450,7 @@
         <v>167</v>
       </c>
       <c r="C129" s="23" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>239</v>
@@ -9467,7 +9466,7 @@
         <v>156</v>
       </c>
       <c r="C130" s="23" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>206</v>
@@ -9483,7 +9482,7 @@
         <v>159</v>
       </c>
       <c r="C131" s="23" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>239</v>
@@ -9499,7 +9498,7 @@
         <v>162</v>
       </c>
       <c r="C132" s="23" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>206</v>
@@ -9515,7 +9514,7 @@
         <v>165</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>239</v>
@@ -9531,7 +9530,7 @@
         <v>169</v>
       </c>
       <c r="C134" s="23" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>206</v>
@@ -9547,7 +9546,7 @@
         <v>172</v>
       </c>
       <c r="C135" s="23" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>239</v>
@@ -9563,7 +9562,7 @@
         <v>176</v>
       </c>
       <c r="C136" s="23" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>206</v>
@@ -9579,7 +9578,7 @@
         <v>180</v>
       </c>
       <c r="C137" s="23" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>239</v>
@@ -9595,7 +9594,7 @@
         <v>183</v>
       </c>
       <c r="C138" s="23" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>239</v>
@@ -9611,7 +9610,7 @@
         <v>186</v>
       </c>
       <c r="C139" s="23" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>206</v>
@@ -9627,7 +9626,7 @@
         <v>189</v>
       </c>
       <c r="C140" s="23" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>206</v>
@@ -9643,7 +9642,7 @@
         <v>192</v>
       </c>
       <c r="C141" s="23" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>206</v>
@@ -9659,7 +9658,7 @@
         <v>195</v>
       </c>
       <c r="C142" s="23" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>206</v>
@@ -9675,7 +9674,7 @@
         <v>86</v>
       </c>
       <c r="C143" s="23" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>239</v>
@@ -9691,7 +9690,7 @@
         <v>89</v>
       </c>
       <c r="C144" s="23" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>239</v>
@@ -9707,7 +9706,7 @@
         <v>91</v>
       </c>
       <c r="C145" s="23" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>239</v>
@@ -9723,7 +9722,7 @@
         <v>94</v>
       </c>
       <c r="C146" s="23" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>206</v>
@@ -9739,7 +9738,7 @@
         <v>97</v>
       </c>
       <c r="C147" s="23" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>206</v>
@@ -9755,7 +9754,7 @@
         <v>100</v>
       </c>
       <c r="C148" s="23" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>206</v>
@@ -9771,7 +9770,7 @@
         <v>104</v>
       </c>
       <c r="C149" s="23" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>206</v>
@@ -9787,7 +9786,7 @@
         <v>107</v>
       </c>
       <c r="C150" s="23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>206</v>
@@ -9803,7 +9802,7 @@
         <v>110</v>
       </c>
       <c r="C151" s="23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>239</v>
@@ -9819,7 +9818,7 @@
         <v>114</v>
       </c>
       <c r="C152" s="23" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>206</v>
@@ -9835,7 +9834,7 @@
         <v>117</v>
       </c>
       <c r="C153" s="23" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>239</v>
@@ -9851,7 +9850,7 @@
         <v>121</v>
       </c>
       <c r="C154" s="23" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D154" s="5" t="s">
         <v>206</v>
@@ -9867,7 +9866,7 @@
         <v>125</v>
       </c>
       <c r="C155" s="23" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D155" s="5" t="s">
         <v>206</v>
@@ -9883,7 +9882,7 @@
         <v>129</v>
       </c>
       <c r="C156" s="23" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D156" s="5" t="s">
         <v>206</v>
@@ -9899,7 +9898,7 @@
         <v>132</v>
       </c>
       <c r="C157" s="23" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D157" s="5" t="s">
         <v>239</v>
@@ -9915,7 +9914,7 @@
         <v>135</v>
       </c>
       <c r="C158" s="23" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D158" s="5" t="s">
         <v>239</v>
@@ -9931,7 +9930,7 @@
         <v>138</v>
       </c>
       <c r="C159" s="23" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D159" s="5" t="s">
         <v>239</v>
@@ -9947,7 +9946,7 @@
         <v>142</v>
       </c>
       <c r="C160" s="23" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D160" s="5" t="s">
         <v>206</v>
@@ -9963,7 +9962,7 @@
         <v>146</v>
       </c>
       <c r="C161" s="23" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D161" s="5" t="s">
         <v>239</v>
@@ -9979,7 +9978,7 @@
         <v>149</v>
       </c>
       <c r="C162" s="23" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D162" s="5" t="s">
         <v>206</v>
@@ -9995,7 +9994,7 @@
         <v>152</v>
       </c>
       <c r="C163" s="23" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D163" s="5" t="s">
         <v>239</v>
@@ -10011,7 +10010,7 @@
         <v>154</v>
       </c>
       <c r="C164" s="23" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="D164" s="5" t="s">
         <v>239</v>
@@ -10027,7 +10026,7 @@
         <v>157</v>
       </c>
       <c r="C165" s="23" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D165" s="5" t="s">
         <v>206</v>
@@ -10043,7 +10042,7 @@
         <v>160</v>
       </c>
       <c r="C166" s="23" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>239</v>
@@ -10059,7 +10058,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="23" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>206</v>
@@ -10075,7 +10074,7 @@
         <v>166</v>
       </c>
       <c r="C168" s="23" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>206</v>
@@ -10091,7 +10090,7 @@
         <v>170</v>
       </c>
       <c r="C169" s="23" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>239</v>
@@ -10107,7 +10106,7 @@
         <v>173</v>
       </c>
       <c r="C170" s="23" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>239</v>
@@ -10123,7 +10122,7 @@
         <v>177</v>
       </c>
       <c r="C171" s="23" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="D171" s="5" t="s">
         <v>206</v>
@@ -10139,7 +10138,7 @@
         <v>181</v>
       </c>
       <c r="C172" s="23" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>239</v>
@@ -10155,7 +10154,7 @@
         <v>184</v>
       </c>
       <c r="C173" s="23" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D173" s="5" t="s">
         <v>206</v>
@@ -10171,7 +10170,7 @@
         <v>187</v>
       </c>
       <c r="C174" s="23" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D174" s="5" t="s">
         <v>239</v>
@@ -10187,7 +10186,7 @@
         <v>190</v>
       </c>
       <c r="C175" s="23" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D175" s="5" t="s">
         <v>239</v>
@@ -10203,7 +10202,7 @@
         <v>193</v>
       </c>
       <c r="C176" s="23" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D176" s="5" t="s">
         <v>206</v>
@@ -10219,7 +10218,7 @@
         <v>196</v>
       </c>
       <c r="C177" s="23" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D177" s="5" t="s">
         <v>239</v>

</xml_diff>

<commit_message>
Refacroting of Simple TC of Lesson 4
</commit_message>
<xml_diff>
--- a/AndyTEST/Libs/SimpleScenariosChecklist_02.xlsx
+++ b/AndyTEST/Libs/SimpleScenariosChecklist_02.xlsx
@@ -3958,8 +3958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4725,8 +4725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F228"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8180,8 +8180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F176"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>